<commit_message>
Added method which finds all available .xlsx files in directory and searches for *report* and *cintorin*
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BOX\eKasa\"/>
     </mc:Choice>
@@ -15,14 +15,14 @@
     <sheet name="Doklady" sheetId="1" r:id="rId1"/>
     <sheet name="Položky dokladu" sheetId="2" r:id="rId2"/>
     <sheet name="Filtrovacie kritériá" sheetId="3" r:id="rId3"/>
-    <sheet name="Sumar" sheetId="4" r:id="rId4"/>
+    <sheet name="Sumar" r:id="rId8" sheetId="4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6675" uniqueCount="1854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6711" uniqueCount="1855">
   <si>
     <t>Dátum zaevidovania v e-kasa</t>
   </si>
@@ -5584,6 +5584,9 @@
   </si>
   <si>
     <t>Položka</t>
+  </si>
+  <si>
+    <t>Uzávierka ku dňu</t>
   </si>
 </sst>
 </file>
@@ -5932,23 +5935,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="42.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="51.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="46.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="37.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="45.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="36.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="34" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="33.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="29.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="29.1796875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="26.1796875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="26.08984375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="42.81640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="51.36328125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.36328125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="23.08984375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.1796875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="15.453125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.453125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="46.36328125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="37.1796875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="45.08984375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="36.08984375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="33.54296875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="29.81640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -33313,17 +33316,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="42.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="6.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="24.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="30" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="45.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="40.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="42.81640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="35.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.1796875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="6.08984375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.90625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="24.90625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="45.08984375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="40.90625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -60214,8 +60217,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.90625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.81640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -60264,22 +60267,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1">
       <c r="A1" t="s">
-        <v>1841</v>
+        <v>1854</v>
       </c>
       <c r="B1" t="s">
         <v>1842</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -60293,79 +60296,80 @@
         <v>1845</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4">
       <c r="A4" t="s">
         <v>1846</v>
       </c>
-      <c r="B4">
-        <v>9039.7000000000062</v>
-      </c>
-      <c r="C4">
+      <c r="B4" t="n">
+        <v>9039.700000000006</v>
+      </c>
+      <c r="C4" t="n">
         <v>7533.0833333333385</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="n">
         <v>1506.6166666666677</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5">
       <c r="A5" t="s">
         <v>1847</v>
       </c>
-      <c r="B5">
-        <v>7.1999999999999993</v>
-      </c>
-      <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5">
+      <c r="B5" t="n">
+        <v>7.199999999999999</v>
+      </c>
+      <c r="C5" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="D5" t="n">
         <v>1.2000000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6">
       <c r="A6" t="s">
         <v>1848</v>
       </c>
-      <c r="B6">
-        <v>20</v>
-      </c>
-      <c r="C6">
+      <c r="B6" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="C6" t="n">
         <v>16.666666666666668</v>
       </c>
-      <c r="D6">
-        <v>3.3333333333333339</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D6" t="n">
+        <v>3.333333333333334</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" t="s">
         <v>1849</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="n">
         <v>10036.200000000006</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="n">
         <v>7555.7500000000055</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="n">
         <v>1511.150000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9">
       <c r="A9" t="s">
         <v>1850</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="n">
         <v>969.3</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="n">
         <v>969.3</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D9"/>
+    </row>
+    <row r="11">
       <c r="A11" t="s">
         <v>1852</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12">
       <c r="A12" t="s">
         <v>1853</v>
       </c>
@@ -60373,39 +60377,39 @@
         <v>1851</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13">
       <c r="A13" t="s">
         <v>370</v>
       </c>
-      <c r="B13">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B13" t="n">
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="14">
       <c r="A14" t="s">
         <v>538</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="n">
         <v>2.4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15">
       <c r="A15" t="s">
         <v>812</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="n">
         <v>19.2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16">
       <c r="A16" t="s">
         <v>844</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="n">
         <v>5.4</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
In exported excel sheet are written counts of individual items and uncategorized items sum and counts
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BOX\eKasa\"/>
     </mc:Choice>
@@ -15,14 +15,14 @@
     <sheet name="Doklady" sheetId="1" r:id="rId1"/>
     <sheet name="Položky dokladu" sheetId="2" r:id="rId2"/>
     <sheet name="Filtrovacie kritériá" sheetId="3" r:id="rId3"/>
-    <sheet name="Sumar" r:id="rId8" sheetId="4"/>
+    <sheet name="Sumar" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6711" uniqueCount="1855">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6679" uniqueCount="1856">
   <si>
     <t>Dátum zaevidovania v e-kasa</t>
   </si>
@@ -5547,9 +5547,6 @@
     <t>Dátum vytvorenia</t>
   </si>
   <si>
-    <t>Uzavierka ku dnu</t>
-  </si>
-  <si>
     <t>31.10.2019 23:59:59.00</t>
   </si>
   <si>
@@ -5587,6 +5584,12 @@
   </si>
   <si>
     <t>Uzávierka ku dňu</t>
+  </si>
+  <si>
+    <t>Jednotková cena</t>
+  </si>
+  <si>
+    <t>Počet položiek</t>
   </si>
 </sst>
 </file>
@@ -5935,23 +5938,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="29.1796875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="26.1796875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="26.08984375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="42.81640625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="51.36328125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="18.36328125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="23.08984375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.1796875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="15.453125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="14.453125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="46.36328125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="37.1796875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="45.08984375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="36.08984375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="33.54296875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="29.81640625" collapsed="true"/>
+    <col min="1" max="1" width="29.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="42.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="51.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="23.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="46.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="37.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="45.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="36.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="33.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="29.81640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -33316,17 +33319,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="42.81640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="35.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.1796875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.08984375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="7.90625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="24.90625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="45.08984375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="40.90625" collapsed="true"/>
+    <col min="1" max="1" width="42.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="24.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="45.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="40.90625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.35">
@@ -60217,8 +60220,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.90625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.81640625" collapsed="true"/>
+    <col min="1" max="1" width="17.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.81640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -60267,149 +60270,209 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="B1" t="s">
-        <v>1842</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
+        <v>1842</v>
+      </c>
+      <c r="C3" t="s">
         <v>1843</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>1844</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>1845</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
+      <c r="B4">
+        <v>9039.7000000000062</v>
+      </c>
+      <c r="C4">
+        <v>7533.0833333333385</v>
+      </c>
+      <c r="D4">
+        <v>1506.6166666666677</v>
+      </c>
+      <c r="E4">
+        <v>2277</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>1846</v>
       </c>
-      <c r="B4" t="n">
-        <v>9039.700000000006</v>
-      </c>
-      <c r="C4" t="n">
-        <v>7533.0833333333385</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1506.6166666666677</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
+      <c r="B5">
+        <v>7.1999999999999993</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>1847</v>
       </c>
-      <c r="B5" t="n">
-        <v>7.199999999999999</v>
-      </c>
-      <c r="C5" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1.2000000000000002</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>16.666666666666668</v>
+      </c>
+      <c r="D6">
+        <v>3.3333333333333339</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>1848</v>
       </c>
-      <c r="B6" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>16.666666666666668</v>
-      </c>
-      <c r="D6" t="n">
-        <v>3.333333333333334</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
+      <c r="B7">
+        <v>10036.200000000006</v>
+      </c>
+      <c r="C7">
+        <v>7555.7500000000055</v>
+      </c>
+      <c r="D7">
+        <v>1511.150000000001</v>
+      </c>
+      <c r="E7">
+        <v>2568</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>1849</v>
       </c>
-      <c r="B7" t="n">
-        <v>10036.200000000006</v>
-      </c>
-      <c r="C7" t="n">
-        <v>7555.7500000000055</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1511.150000000001</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
+      <c r="B9">
+        <v>969.3</v>
+      </c>
+      <c r="C9">
+        <v>969.3</v>
+      </c>
+      <c r="E9">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>1852</v>
+      </c>
+      <c r="B12" t="s">
         <v>1850</v>
       </c>
-      <c r="B9" t="n">
-        <v>969.3</v>
-      </c>
-      <c r="C9" t="n">
-        <v>969.3</v>
-      </c>
-      <c r="D9"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>1852</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>1853</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1851</v>
-      </c>
-    </row>
-    <row r="13">
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1854</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>370</v>
       </c>
-      <c r="B13" t="n">
-        <v>15.0</v>
-      </c>
-    </row>
-    <row r="14">
+      <c r="B13">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>538</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="15">
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>0.19999999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>812</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>19.2</v>
       </c>
-    </row>
-    <row r="16">
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>844</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>5.4</v>
       </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>1848</v>
+      </c>
+      <c r="B17">
+        <v>41.999999999999993</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>